<commit_message>
Proper decode working on hardware I think
</commit_message>
<xml_diff>
--- a/excel/mode_s_frame_analysis.xlsx
+++ b/excel/mode_s_frame_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B791459-9744-424B-A9E6-DEE722C46551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7344737-7784-4B90-8260-9A8B47510908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28640" yWindow="-4360" windowWidth="21780" windowHeight="9980" xr2:uid="{93B0C022-ACAC-4012-B936-897677000189}"/>
+    <workbookView xWindow="-28080" yWindow="-3800" windowWidth="21780" windowHeight="9980" xr2:uid="{93B0C022-ACAC-4012-B936-897677000189}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Value (Dec)</t>
   </si>
@@ -81,7 +81,31 @@
     <t>3c</t>
   </si>
   <si>
-    <t>ab</t>
+    <t>Binary Words</t>
+  </si>
+  <si>
+    <t>Hex Words</t>
+  </si>
+  <si>
+    <t>9e</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Desired</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Binary</t>
   </si>
 </sst>
 </file>
@@ -146,18 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -165,6 +183,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159B8FA0-5B08-4D2C-A59A-32ED82D46FEA}">
-  <dimension ref="A2:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -492,34 +515,39 @@
     <col min="3" max="3" width="3.7890625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1">
+        <v>1010</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H2" t="str">
         <f>BIN2HEX(H1)</f>
-        <v>0</v>
+        <v>A</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
@@ -538,85 +566,91 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <f>B4--1</f>
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <f>C4-B4</f>
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <f t="shared" ref="D5:H5" si="0">D4-C4</f>
         <v>8</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>-31</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="8"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="6">
         <v>17</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>5</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" t="s">
-        <v>15</v>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="str">
@@ -640,64 +674,100 @@
         <v>11101111</v>
       </c>
       <c r="G9" t="e">
-        <f t="shared" ref="C9:H9" si="2">DEC2BIN(G8, G5)</f>
+        <f t="shared" ref="G9:H9" si="2">DEC2BIN(G8, G5)</f>
         <v>#NUM!</v>
       </c>
       <c r="H9" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
       <c r="L9" t="str">
-        <f>HEX2BIN(L8)</f>
-        <v>111100</v>
+        <f>HEX2BIN(L8,8)</f>
+        <v>00000001</v>
       </c>
       <c r="M9" t="str">
-        <f>HEX2BIN(M8)</f>
-        <v>10101011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="4" t="str">
+        <f>HEX2BIN(M8,8)</f>
+        <v>10011110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="str">
         <f>_xlfn.CONCAT(B9,C9)</f>
         <v>10001101</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" t="str">
+      <c r="C10" s="9"/>
+      <c r="D10" s="1" t="str">
         <f>D9</f>
         <v>10101011</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E10" s="1" t="str">
         <f>E9</f>
         <v>11001101</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F10" s="1" t="str">
         <f>F9</f>
         <v>11101111</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="4" t="str">
-        <f>BIN2HEX(B11)</f>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9" t="str">
+        <f>BIN2HEX(B10)</f>
         <v>8D</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" t="str">
-        <f>BIN2HEX(D11)</f>
+      <c r="C11" s="9"/>
+      <c r="D11" s="1" t="str">
+        <f>BIN2HEX(D10)</f>
         <v>AB</v>
       </c>
-      <c r="E12" t="str">
-        <f t="shared" ref="E12:F12" si="3">BIN2HEX(E11)</f>
+      <c r="E11" s="1" t="str">
+        <f t="shared" ref="E11:F11" si="3">BIN2HEX(E10)</f>
         <v>CD</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F11" s="1" t="str">
         <f t="shared" si="3"/>
         <v>EF</v>
       </c>
+      <c r="L11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="str">
+        <f>HEX2BIN(L12,8)</f>
+        <v>00000011</v>
+      </c>
+      <c r="M13" t="str">
+        <f>HEX2BIN(M12,8)</f>
+        <v>00111100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add bodge board for post-detector amplifier
</commit_message>
<xml_diff>
--- a/excel/mode_s_frame_analysis.xlsx
+++ b/excel/mode_s_frame_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7344737-7784-4B90-8260-9A8B47510908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876ACC75-DF46-4C84-B6F4-7946DF775499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28080" yWindow="-3800" windowWidth="21780" windowHeight="9980" xr2:uid="{93B0C022-ACAC-4012-B936-897677000189}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="9984" xr2:uid="{93B0C022-ACAC-4012-B936-897677000189}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -183,11 +183,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +504,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -642,10 +641,10 @@
       <c r="K8" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -694,7 +693,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="9" t="str">
@@ -716,7 +715,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="9" t="str">
@@ -744,10 +743,10 @@
       <c r="K12" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="8" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>